<commit_message>
Final Changes Before Demo
Applied new skills dropdown values, removed signon credentials for security, and cleaned up data load scripts for team members, roles, and products.
</commit_message>
<xml_diff>
--- a/data_to_load/products.xlsx
+++ b/data_to_load/products.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krpop\Documents\KenP\Applications-Python\demand_capacity_app\data_to_load\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krpop\Documents\KenP\Applications-Python\demand-capacity2\data_to_load\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BD15C26-DCF2-44E3-B28F-36D93BF4198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B26B1DD-2A30-44CF-94DE-DAA1A4A30014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{AB67AD10-3DEB-4CC1-9CD2-9CE7B80EC845}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="11440" xr2:uid="{AB67AD10-3DEB-4CC1-9CD2-9CE7B80EC845}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="62">
   <si>
     <t>Compliance Companion</t>
   </si>
@@ -204,181 +204,25 @@
     <t>technology_executive</t>
   </si>
   <si>
-    <t>Production Operation Support</t>
-  </si>
-  <si>
-    <t>Observability</t>
-  </si>
-  <si>
-    <t>B2B webMethods HA Setup</t>
-  </si>
-  <si>
-    <t>Value Chain webMethods Stack Upgrade / HA Setup</t>
-  </si>
-  <si>
-    <t>Kafka UI to Kafka Bat</t>
-  </si>
-  <si>
-    <t>JWKS Edge Migration</t>
-  </si>
-  <si>
-    <t>AWS Optimization / Housekeeping</t>
-  </si>
-  <si>
-    <t>Jenkin Upgrade</t>
-  </si>
-  <si>
-    <t>API Call Log Observability</t>
-  </si>
-  <si>
-    <t>Security Enhancements</t>
-  </si>
-  <si>
-    <t xml:space="preserve">API Management </t>
-  </si>
-  <si>
-    <t>API Self-Service (Developer Apps / API Keys / Proxies)</t>
-  </si>
-  <si>
-    <t>MAGIC API to Native JWT</t>
-  </si>
-  <si>
-    <t>KeyBridge (CAS)</t>
-  </si>
-  <si>
-    <t>Event Driven Architecture</t>
-  </si>
-  <si>
-    <t>Common framework assets</t>
-  </si>
-  <si>
-    <t>Platform readiness for Camel Deployments - GCP</t>
-  </si>
-  <si>
-    <t>Schema Registry Optimizations &amp; Enhancements</t>
-  </si>
-  <si>
-    <t>Airflow MFT (Phase 1)</t>
-  </si>
-  <si>
-    <t>PLM Upgrade (Camel Migration Phase 1)</t>
-  </si>
-  <si>
-    <t>STARLiMS Upgrade</t>
-  </si>
-  <si>
-    <t>ftp to sftp migration</t>
-  </si>
-  <si>
-    <t>JDE Upgrade Problem Resolution Support</t>
-  </si>
-  <si>
-    <t>WMS Upgrade</t>
-  </si>
-  <si>
-    <t>ANA AS400 Decomm</t>
-  </si>
-  <si>
-    <t>Mongolia Work Order</t>
-  </si>
-  <si>
-    <t>Central Asia Debit Card integration to EBS</t>
-  </si>
-  <si>
-    <t>Order Trace Application Enhancement</t>
-  </si>
-  <si>
-    <t>OneSource for Global Trade</t>
-  </si>
-  <si>
-    <t>Legacy 3 Replacement</t>
-  </si>
-  <si>
-    <t>Integration assessment / Migration</t>
-  </si>
-  <si>
-    <t>Hybris CA UM to Kafka Migration</t>
-  </si>
-  <si>
-    <t>Project Ocean</t>
-  </si>
-  <si>
-    <t>Poland E-Invoice</t>
-  </si>
-  <si>
-    <t>Taiwan Payment Gateway</t>
-  </si>
-  <si>
-    <t>Philipines MEP Kafka</t>
-  </si>
-  <si>
-    <t>Vietnam Invoice Legal Requirement</t>
-  </si>
-  <si>
-    <t>NextGen Commerce</t>
-  </si>
-  <si>
-    <t>NextGen IMS/OMS</t>
-  </si>
-  <si>
-    <t>NextGen MLP 1.0</t>
-  </si>
-  <si>
-    <t>MecuryGate CW</t>
-  </si>
-  <si>
-    <t>Central Asia Enhancement</t>
-  </si>
-  <si>
-    <t>Europe Enhancement</t>
-  </si>
-  <si>
-    <t>LATAM MDMS</t>
-  </si>
-  <si>
-    <t>MEP India and Central Asia (Including Kafka Enablement )</t>
-  </si>
-  <si>
-    <t>Central Asia - Kyrgyzstan Market launch</t>
-  </si>
-  <si>
-    <t>Ken Popkin</t>
-  </si>
-  <si>
-    <t>Manish Sannat</t>
-  </si>
-  <si>
-    <t>Sayan Chakraborty</t>
-  </si>
-  <si>
-    <t>Ryan Vetter</t>
-  </si>
-  <si>
-    <t>Smiti Majumdar</t>
-  </si>
-  <si>
-    <t>Darrell Tanis</t>
-  </si>
-  <si>
-    <t>Cliff Seow</t>
-  </si>
-  <si>
-    <t>Mike Heyn</t>
-  </si>
-  <si>
-    <t>Srikanth Prathipati</t>
-  </si>
-  <si>
-    <t>Karthik Ramasamy</t>
-  </si>
-  <si>
-    <t>Nancy Wong</t>
-  </si>
-  <si>
-    <t>Renuka Dabas</t>
-  </si>
-  <si>
     <t>Gaurav Vijaywargia</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>Manish</t>
+  </si>
+  <si>
+    <t>Sayan</t>
+  </si>
+  <si>
+    <t>Ryan</t>
+  </si>
+  <si>
+    <t>Smiti</t>
+  </si>
+  <si>
+    <t>Darrell</t>
   </si>
 </sst>
 </file>
@@ -402,15 +246,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -441,23 +283,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -799,76 +638,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AF76323-1EAE-4C92-B7E3-4134B929D9C5}">
-  <dimension ref="A1:C69"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C71" sqref="C71"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18.90625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.6328125" style="2"/>
+    <col min="1" max="1" width="49.08984375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21" style="4" customWidth="1"/>
+    <col min="3" max="3" width="18.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.6328125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>113</v>
+      <c r="B2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>113</v>
+      <c r="B3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>113</v>
+      <c r="B4" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>113</v>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -876,10 +715,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -887,10 +726,10 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -898,10 +737,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -909,10 +748,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -920,10 +759,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -931,10 +770,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -942,10 +781,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -953,10 +792,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -964,10 +803,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -975,21 +814,21 @@
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -997,10 +836,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -1008,10 +847,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -1019,10 +858,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -1030,10 +869,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -1041,10 +880,10 @@
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -1052,10 +891,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -1063,471 +902,18 @@
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>106</v>
+        <v>61</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B37" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A39" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B39" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A40" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B40" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A41" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B41" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A42" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" t="s">
-        <v>110</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B43" t="s">
-        <v>110</v>
-      </c>
-      <c r="C43" s="6"/>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B44" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44" s="6"/>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="B45" t="s">
-        <v>110</v>
-      </c>
-      <c r="C45" s="6"/>
-    </row>
-    <row r="46" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B46" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46" s="6"/>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A47" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="B47" t="s">
-        <v>110</v>
-      </c>
-      <c r="C47" s="6"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A48" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B48" t="s">
-        <v>110</v>
-      </c>
-      <c r="C48" s="6"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49" t="s">
-        <v>110</v>
-      </c>
-      <c r="C49" s="6"/>
-    </row>
-    <row r="50" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A50" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B50" t="s">
-        <v>110</v>
-      </c>
-      <c r="C50" s="6"/>
-    </row>
-    <row r="51" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B51" t="s">
-        <v>110</v>
-      </c>
-      <c r="C51" s="6"/>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A52" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B52" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="6"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B53" t="s">
-        <v>110</v>
-      </c>
-      <c r="C53" s="6"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A54" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A55" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C55" s="6"/>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A56" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="B56" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C56" s="6"/>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A57" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="B57" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C57" s="6"/>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A58" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="B58" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C58" s="6"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A59" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="B59" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C59" s="6"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A60" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="B60" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C60" s="6"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A61" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="B61" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C61" s="6"/>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B62" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C62" s="6"/>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A63" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B63" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C63" s="6"/>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A64" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B64" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C64" s="6"/>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B65" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C65" s="6"/>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C66" s="6"/>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B67" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C67" s="6"/>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C68" s="6"/>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C69" s="6"/>
+        <v>55</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C24">
-    <sortCondition ref="A2:A24"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C3">
+    <sortCondition ref="A2:A3"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1736,6 +1122,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010086A72C854002854794493D02C0B42ECC" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b7c05f9d745027607f7cc13caf7a7fc2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="95b0fa68-fb80-4536-975a-110ff333bd9a" xmlns:ns3="3f5717c7-db0b-4217-ba9d-d939c34275cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="71bac019da2bb0526f6d7cdd3dc708b4" ns2:_="" ns3:_="">
     <xsd:import namespace="95b0fa68-fb80-4536-975a-110ff333bd9a"/>
@@ -1990,15 +1385,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DADFDD51-E98C-4A2F-9DC1-81CEE9EC7660}">
   <ds:schemaRefs>
@@ -2017,6 +1403,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D551748C-E602-4AD2-AEB2-C933215C0BFC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5369BF68-05DD-4C76-9062-179DEE4E2A9E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2033,12 +1427,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D551748C-E602-4AD2-AEB2-C933215C0BFC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>